<commit_message>
Completada la trazabilidad de tablas de app web
</commit_message>
<xml_diff>
--- a/docs/diseno/trazabilidad-tablas.xlsx
+++ b/docs/diseno/trazabilidad-tablas.xlsx
@@ -22,6 +22,87 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
+    <t xml:space="preserve">ECU-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU-027</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARCHIVO</t>
   </si>
   <si>
@@ -92,87 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">TURNO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECU027</t>
   </si>
 </sst>
 </file>
@@ -273,20 +273,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:Y1"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7959183673469"/>
-    <col collapsed="false" hidden="false" max="25" min="2" style="0" width="4.11224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.219387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="2" style="0" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="84.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -359,140 +359,200 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V24" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
         <v>50</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporada trazabilidad de tablas Terminal
</commit_message>
<xml_diff>
--- a/docs/diseno/trazabilidad-tablas.xlsx
+++ b/docs/diseno/trazabilidad-tablas.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="webapp" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="terminal" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="pago" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t xml:space="preserve">ECU-001</t>
   </si>
@@ -182,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -203,6 +205,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,12 +256,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,97 +292,102 @@
   </sheetPr>
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF13" activeCellId="0" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.219387755102"/>
-    <col collapsed="false" hidden="false" max="28" min="2" style="0" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="20" min="6" style="0" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="28" min="23" style="0" width="2.81632653061224"/>
     <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -373,7 +395,7 @@
       <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -386,7 +408,7 @@
       <c r="A4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -424,10 +446,13 @@
       <c r="A11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U11" s="0" t="n">
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -435,13 +460,13 @@
       <c r="A12" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" s="0" t="n">
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -469,16 +494,16 @@
       <c r="A17" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="V17" s="0" t="n">
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -491,10 +516,10 @@
       <c r="A19" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U19" s="0" t="n">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -502,10 +527,10 @@
       <c r="A20" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U20" s="0" t="n">
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -513,10 +538,10 @@
       <c r="A21" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U21" s="0" t="n">
+      <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -524,7 +549,7 @@
       <c r="A22" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="V22" s="0" t="n">
+      <c r="V22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -537,10 +562,10 @@
       <c r="A24" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="V24" s="0" t="n">
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -548,10 +573,10 @@
       <c r="A25" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U25" s="0" t="n">
+      <c r="B25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -564,4 +589,788 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AB25"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.219387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="2" style="0" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>